<commit_message>
Clean up on input data for assignment problems
</commit_message>
<xml_diff>
--- a/Misc/2019_20-Even-18CS42-DAA-Lecture-Plan.xlsx
+++ b/Misc/2019_20-Even-18CS42-DAA-Lecture-Plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ramrustagi/Projects/github/2019_20-Even-18CS42-DAA/Misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E498AE6D-E6AA-E842-865B-85C7A7ADB688}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{762EA614-3633-7C42-B865-B95740BA2674}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8460" yWindow="460" windowWidth="17140" windowHeight="15540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1340" yWindow="460" windowWidth="20700" windowHeight="15540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="COs" sheetId="2" r:id="rId1"/>
@@ -866,7 +866,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -889,23 +889,9 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -931,16 +917,33 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1306,7 +1309,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1367,7 +1370,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1785,10 +1788,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:F81"/>
+  <dimension ref="A2:H81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1796,893 +1799,918 @@
     <col min="1" max="1" width="6.5" style="5" customWidth="1"/>
     <col min="2" max="2" width="6.1640625" style="5" customWidth="1"/>
     <col min="3" max="3" width="54.1640625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="76.33203125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="11" style="32" customWidth="1"/>
     <col min="5" max="5" width="6.5" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.1640625" style="8" customWidth="1"/>
     <col min="7" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="12"/>
+      <c r="D2" s="26"/>
       <c r="E2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="13"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="21">
+      <c r="F2" s="12"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="15">
         <v>1</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="28" t="s">
+      <c r="D3" s="27"/>
+      <c r="E3" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="30" t="s">
+      <c r="F3" s="22" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="21">
+      <c r="H3" s="2">
+        <f>13/38</f>
+        <v>0.34210526315789475</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="15">
         <v>2</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="D4" s="14"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="31"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="21">
+      <c r="D4" s="28"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="23"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="15">
         <v>3</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="D5" s="14"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="31"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D6" s="14"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="31"/>
-    </row>
-    <row r="7" spans="1:6" ht="34" x14ac:dyDescent="0.25">
-      <c r="A7" s="21">
+      <c r="D5" s="28"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="23"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D6" s="28"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="23"/>
+    </row>
+    <row r="7" spans="1:8" ht="34" x14ac:dyDescent="0.25">
+      <c r="A7" s="15">
         <v>4</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="28" t="s">
+      <c r="D7" s="28"/>
+      <c r="E7" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="30" t="s">
+      <c r="F7" s="22" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="34" x14ac:dyDescent="0.25">
-      <c r="A8" s="21">
+    <row r="8" spans="1:8" ht="34" x14ac:dyDescent="0.25">
+      <c r="A8" s="15">
         <v>5</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="30"/>
-    </row>
-    <row r="9" spans="1:6" ht="34" x14ac:dyDescent="0.25">
-      <c r="A9" s="21">
+      <c r="D8" s="28"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="22"/>
+    </row>
+    <row r="9" spans="1:8" ht="34" x14ac:dyDescent="0.25">
+      <c r="A9" s="15">
         <v>6</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="23" t="s">
+      <c r="C9" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="D9" s="14"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="31"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D9" s="28"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="23"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="31"/>
-    </row>
-    <row r="11" spans="1:6" ht="34" x14ac:dyDescent="0.25">
-      <c r="A11" s="21">
+      <c r="D10" s="29"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="23"/>
+    </row>
+    <row r="11" spans="1:8" ht="34" x14ac:dyDescent="0.25">
+      <c r="A11" s="15">
         <v>7</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="28" t="s">
+      <c r="D11" s="28"/>
+      <c r="E11" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="30" t="s">
+      <c r="F11" s="22" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="34" x14ac:dyDescent="0.25">
-      <c r="A12" s="21">
+    <row r="12" spans="1:8" ht="34" x14ac:dyDescent="0.25">
+      <c r="A12" s="15">
         <v>8</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="23" t="s">
+      <c r="C12" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="30"/>
-    </row>
-    <row r="13" spans="1:6" ht="35" x14ac:dyDescent="0.25">
-      <c r="A13" s="21">
+      <c r="D12" s="28"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="22"/>
+    </row>
+    <row r="13" spans="1:8" ht="35" x14ac:dyDescent="0.25">
+      <c r="A13" s="15">
         <v>9</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="24" t="s">
+      <c r="C13" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="D13" s="17"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="30"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D13" s="30"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="22"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="31"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="21">
+      <c r="D14" s="29"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="23"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="15">
         <v>10</v>
       </c>
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="24" t="s">
+      <c r="C15" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="D15" s="17"/>
-      <c r="E15" s="28" t="s">
+      <c r="D15" s="30"/>
+      <c r="E15" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="F15" s="30" t="s">
+      <c r="F15" s="22" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="21">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="15">
         <v>11</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="23" t="s">
+      <c r="C16" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="D16" s="14"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="30"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="22"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="21">
+      <c r="A17" s="15">
         <v>12</v>
       </c>
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="23" t="s">
+      <c r="C17" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="14"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="30"/>
+      <c r="D17" s="28">
+        <f>12/38</f>
+        <v>0.31578947368421051</v>
+      </c>
+      <c r="E17" s="24"/>
+      <c r="F17" s="22"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="29"/>
-      <c r="F18" s="31"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="23"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="21">
+      <c r="A19" s="15">
         <v>13</v>
       </c>
-      <c r="B19" s="21" t="s">
+      <c r="B19" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="24" t="s">
+      <c r="C19" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="D19" s="17"/>
-      <c r="E19" s="28" t="s">
+      <c r="D19" s="30">
+        <f>13/38</f>
+        <v>0.34210526315789475</v>
+      </c>
+      <c r="E19" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="F19" s="30" t="s">
+      <c r="F19" s="22" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="21">
+      <c r="A20" s="15">
         <v>14</v>
       </c>
-      <c r="B20" s="21" t="s">
+      <c r="B20" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="24" t="s">
+      <c r="C20" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="D20" s="17"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="30"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="22"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="21">
+      <c r="A21" s="15">
         <v>15</v>
       </c>
-      <c r="B21" s="21" t="s">
+      <c r="B21" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="24" t="s">
+      <c r="C21" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="D21" s="17"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="30"/>
+      <c r="D21" s="30">
+        <f>15/38</f>
+        <v>0.39473684210526316</v>
+      </c>
+      <c r="E21" s="24"/>
+      <c r="F21" s="22"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="29"/>
-      <c r="F22" s="31"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="23"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="21">
+      <c r="A23" s="15">
         <v>16</v>
       </c>
-      <c r="B23" s="25" t="s">
+      <c r="B23" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="24" t="s">
+      <c r="C23" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="D23" s="17"/>
-      <c r="E23" s="28" t="s">
+      <c r="D23" s="30"/>
+      <c r="E23" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="F23" s="30" t="s">
+      <c r="F23" s="22" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="21">
+      <c r="A24" s="15">
         <v>17</v>
       </c>
-      <c r="B24" s="25" t="s">
+      <c r="B24" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="26" t="s">
+      <c r="C24" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="D24" s="18"/>
-      <c r="E24" s="29"/>
-      <c r="F24" s="31"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="23"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="21">
+      <c r="A25" s="15">
         <v>18</v>
       </c>
-      <c r="B25" s="25" t="s">
+      <c r="B25" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="24" t="s">
+      <c r="C25" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="D25" s="17"/>
-      <c r="E25" s="29"/>
-      <c r="F25" s="31"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="23"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="31"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="23"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="21">
+      <c r="A27" s="15">
         <v>19</v>
       </c>
-      <c r="B27" s="25" t="s">
+      <c r="B27" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C27" s="24" t="s">
+      <c r="C27" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="D27" s="17"/>
-      <c r="E27" s="28" t="s">
+      <c r="D27" s="30"/>
+      <c r="E27" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F27" s="30" t="s">
+      <c r="F27" s="22" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="21">
+      <c r="A28" s="15">
         <v>20</v>
       </c>
-      <c r="B28" s="25" t="s">
+      <c r="B28" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C28" s="24" t="s">
+      <c r="C28" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="D28" s="17"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="31"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="23"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="21">
+      <c r="A29" s="15">
         <v>21</v>
       </c>
-      <c r="B29" s="25" t="s">
+      <c r="B29" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C29" s="24" t="s">
+      <c r="C29" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="D29" s="17"/>
-      <c r="E29" s="29"/>
-      <c r="F29" s="31"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="23"/>
     </row>
     <row r="30" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="29"/>
-      <c r="F30" s="31"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="25"/>
+      <c r="F30" s="23"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="21">
+      <c r="A31" s="15">
         <v>22</v>
       </c>
-      <c r="B31" s="25" t="s">
+      <c r="B31" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C31" s="24" t="s">
+      <c r="C31" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="D31" s="17"/>
-      <c r="E31" s="28" t="s">
+      <c r="D31" s="30"/>
+      <c r="E31" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="F31" s="30" t="s">
+      <c r="F31" s="22" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="21">
+      <c r="A32" s="15">
         <v>23</v>
       </c>
-      <c r="B32" s="21" t="s">
+      <c r="B32" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C32" s="24" t="s">
+      <c r="C32" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="D32" s="17"/>
-      <c r="E32" s="29"/>
-      <c r="F32" s="31"/>
+      <c r="D32" s="30"/>
+      <c r="E32" s="25"/>
+      <c r="F32" s="23"/>
     </row>
     <row r="33" spans="1:6" ht="35" x14ac:dyDescent="0.25">
-      <c r="A33" s="21">
+      <c r="A33" s="15">
         <v>24</v>
       </c>
-      <c r="B33" s="21" t="s">
+      <c r="B33" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C33" s="24" t="s">
+      <c r="C33" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="D33" s="17"/>
-      <c r="E33" s="29"/>
-      <c r="F33" s="31"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="25"/>
+      <c r="F33" s="23"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
-      <c r="D34" s="16"/>
-      <c r="E34" s="29"/>
-      <c r="F34" s="31"/>
+      <c r="D34" s="29"/>
+      <c r="E34" s="25"/>
+      <c r="F34" s="23"/>
     </row>
     <row r="35" spans="1:6" ht="35" x14ac:dyDescent="0.25">
-      <c r="A35" s="21">
+      <c r="A35" s="15">
         <v>25</v>
       </c>
-      <c r="B35" s="21" t="s">
+      <c r="B35" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C35" s="24" t="s">
+      <c r="C35" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="D35" s="17"/>
-      <c r="E35" s="28" t="s">
+      <c r="D35" s="30"/>
+      <c r="E35" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="F35" s="30" t="s">
+      <c r="F35" s="22" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="21">
+      <c r="A36" s="15">
         <v>26</v>
       </c>
-      <c r="B36" s="21" t="s">
+      <c r="B36" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C36" s="24" t="s">
+      <c r="C36" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="D36" s="17"/>
-      <c r="E36" s="29"/>
-      <c r="F36" s="31"/>
+      <c r="D36" s="30"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="23"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="21">
+      <c r="A37" s="15">
         <v>27</v>
       </c>
-      <c r="B37" s="21" t="s">
+      <c r="B37" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C37" s="24" t="s">
+      <c r="C37" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="D37" s="17"/>
-      <c r="E37" s="29"/>
-      <c r="F37" s="31"/>
+      <c r="D37" s="30"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="23"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="16"/>
-      <c r="E38" s="29"/>
-      <c r="F38" s="31"/>
+      <c r="D38" s="29"/>
+      <c r="E38" s="25"/>
+      <c r="F38" s="23"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="21">
+      <c r="A39" s="15">
         <v>28</v>
       </c>
-      <c r="B39" s="21" t="s">
+      <c r="B39" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C39" s="24" t="s">
+      <c r="C39" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="D39" s="17"/>
-      <c r="E39" s="28" t="s">
+      <c r="D39" s="30"/>
+      <c r="E39" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="F39" s="30" t="s">
+      <c r="F39" s="22" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="21">
+      <c r="A40" s="15">
         <v>29</v>
       </c>
-      <c r="B40" s="21" t="s">
+      <c r="B40" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C40" s="24" t="s">
+      <c r="C40" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="D40" s="17"/>
-      <c r="E40" s="29"/>
-      <c r="F40" s="31"/>
+      <c r="D40" s="30"/>
+      <c r="E40" s="25"/>
+      <c r="F40" s="23"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="21">
+      <c r="A41" s="15">
         <v>30</v>
       </c>
-      <c r="B41" s="21" t="s">
+      <c r="B41" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C41" s="24" t="s">
+      <c r="C41" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="D41" s="17"/>
-      <c r="E41" s="29"/>
-      <c r="F41" s="31"/>
+      <c r="D41" s="30"/>
+      <c r="E41" s="25"/>
+      <c r="F41" s="23"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
-      <c r="D42" s="16"/>
-      <c r="E42" s="29"/>
-      <c r="F42" s="31"/>
+      <c r="D42" s="29"/>
+      <c r="E42" s="25"/>
+      <c r="F42" s="23"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="21">
+      <c r="A43" s="15">
         <v>31</v>
       </c>
-      <c r="B43" s="21" t="s">
+      <c r="B43" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C43" s="24" t="s">
+      <c r="C43" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="D43" s="17"/>
-      <c r="E43" s="28" t="s">
+      <c r="D43" s="30"/>
+      <c r="E43" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="F43" s="30" t="s">
+      <c r="F43" s="22" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="21">
+      <c r="A44" s="15">
         <v>32</v>
       </c>
-      <c r="B44" s="21" t="s">
+      <c r="B44" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C44" s="24" t="s">
+      <c r="C44" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="D44" s="17"/>
-      <c r="E44" s="29"/>
-      <c r="F44" s="31"/>
+      <c r="D44" s="30"/>
+      <c r="E44" s="25"/>
+      <c r="F44" s="23"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="21">
+      <c r="A45" s="15">
         <v>33</v>
       </c>
-      <c r="B45" s="21" t="s">
+      <c r="B45" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C45" s="24" t="s">
+      <c r="C45" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D45" s="17"/>
-      <c r="E45" s="29"/>
-      <c r="F45" s="31"/>
+      <c r="D45" s="30"/>
+      <c r="E45" s="25"/>
+      <c r="F45" s="23"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="7"/>
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
-      <c r="D46" s="16"/>
-      <c r="E46" s="29"/>
-      <c r="F46" s="31"/>
+      <c r="D46" s="29"/>
+      <c r="E46" s="25"/>
+      <c r="F46" s="23"/>
     </row>
     <row r="47" spans="1:6" ht="35" x14ac:dyDescent="0.25">
-      <c r="A47" s="21">
+      <c r="A47" s="15">
         <v>34</v>
       </c>
-      <c r="B47" s="21" t="s">
+      <c r="B47" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C47" s="24" t="s">
+      <c r="C47" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="D47" s="17"/>
-      <c r="E47" s="28" t="s">
+      <c r="D47" s="30"/>
+      <c r="E47" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="F47" s="30" t="s">
+      <c r="F47" s="22" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="21">
+      <c r="A48" s="15">
         <v>35</v>
       </c>
-      <c r="B48" s="21" t="s">
+      <c r="B48" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C48" s="24" t="s">
+      <c r="C48" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="D48" s="17"/>
-      <c r="E48" s="29"/>
-      <c r="F48" s="31"/>
+      <c r="D48" s="30"/>
+      <c r="E48" s="25"/>
+      <c r="F48" s="23"/>
     </row>
     <row r="49" spans="1:6" ht="35" x14ac:dyDescent="0.25">
-      <c r="A49" s="21">
+      <c r="A49" s="15">
         <v>36</v>
       </c>
-      <c r="B49" s="21" t="s">
+      <c r="B49" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C49" s="24" t="s">
+      <c r="C49" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="D49" s="17"/>
-      <c r="E49" s="29"/>
-      <c r="F49" s="31"/>
+      <c r="D49" s="30"/>
+      <c r="E49" s="25"/>
+      <c r="F49" s="23"/>
     </row>
     <row r="50" spans="1:6" ht="52" x14ac:dyDescent="0.25">
-      <c r="A50" s="21">
+      <c r="A50" s="15">
         <v>37</v>
       </c>
-      <c r="B50" s="21" t="s">
+      <c r="B50" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C50" s="24" t="s">
+      <c r="C50" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="D50" s="17"/>
-      <c r="E50" s="29"/>
-      <c r="F50" s="31"/>
+      <c r="D50" s="30"/>
+      <c r="E50" s="25"/>
+      <c r="F50" s="23"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
-      <c r="D51" s="16"/>
+      <c r="D51" s="29"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="D52" s="14"/>
+      <c r="D52" s="28"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="21" t="s">
+      <c r="A53" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="B53" s="21" t="s">
+      <c r="B53" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C53" s="23" t="s">
+      <c r="C53" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D53" s="14"/>
+      <c r="D53" s="28"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="21" t="s">
+      <c r="A54" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="B54" s="21" t="s">
+      <c r="B54" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C54" s="23" t="s">
+      <c r="C54" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="D54" s="14"/>
+      <c r="D54" s="28"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="21" t="s">
+      <c r="A55" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="B55" s="21" t="s">
+      <c r="B55" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C55" s="23" t="s">
+      <c r="C55" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="D55" s="14"/>
+      <c r="D55" s="28"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="21" t="s">
+      <c r="A56" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="B56" s="21" t="s">
+      <c r="B56" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C56" s="23" t="s">
+      <c r="C56" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="D56" s="14"/>
+      <c r="D56" s="28"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="21" t="s">
+      <c r="A57" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="B57" s="21" t="s">
+      <c r="B57" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C57" s="23" t="s">
+      <c r="C57" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="D57" s="14"/>
+      <c r="D57" s="28"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="21" t="s">
+      <c r="A58" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="B58" s="25" t="s">
+      <c r="B58" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C58" s="23" t="s">
+      <c r="C58" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="D58" s="14"/>
+      <c r="D58" s="28"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="21" t="s">
+      <c r="A59" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="B59" s="21" t="s">
+      <c r="B59" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C59" s="23" t="s">
+      <c r="C59" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="D59" s="14"/>
+      <c r="D59" s="28"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="27" t="s">
+      <c r="A60" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="B60" s="21" t="s">
+      <c r="B60" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C60" s="23" t="s">
+      <c r="C60" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="D60" s="14"/>
+      <c r="D60" s="28"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="21" t="s">
+      <c r="A61" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="B61" s="21" t="s">
+      <c r="B61" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C61" s="23" t="s">
+      <c r="C61" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="D61" s="14"/>
+      <c r="D61" s="28"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="21" t="s">
+      <c r="A62" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="B62" s="21" t="s">
+      <c r="B62" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C62" s="23" t="s">
+      <c r="C62" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="D62" s="14"/>
+      <c r="D62" s="28"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="21" t="s">
+      <c r="A63" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="B63" s="21" t="s">
+      <c r="B63" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C63" s="23" t="s">
+      <c r="C63" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="D63" s="14"/>
+      <c r="D63" s="28"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="21" t="s">
+      <c r="A64" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="B64" s="21" t="s">
+      <c r="B64" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="C64" s="23" t="s">
+      <c r="C64" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D64" s="14"/>
+      <c r="D64" s="28"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="21" t="s">
+      <c r="A65" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="B65" s="21"/>
-      <c r="C65" s="23"/>
-      <c r="D65" s="14"/>
+      <c r="B65" s="15"/>
+      <c r="C65" s="17"/>
+      <c r="D65" s="28"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D66" s="14"/>
+      <c r="D66" s="28"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D67" s="14"/>
+      <c r="D67" s="28"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D68" s="14"/>
+      <c r="D68" s="28"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D69" s="14"/>
+      <c r="D69" s="28"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D70" s="14"/>
+      <c r="D70" s="28"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D71" s="14"/>
+      <c r="D71" s="28"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D72" s="14"/>
+      <c r="D72" s="28"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D73" s="14"/>
+      <c r="D73" s="28"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D74" s="14"/>
+      <c r="D74" s="28"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D75" s="14"/>
+      <c r="D75" s="28"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D76" s="14"/>
+      <c r="D76" s="28"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D77" s="14"/>
+      <c r="D77" s="28"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D78" s="14"/>
+      <c r="D78" s="28"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D79" s="14"/>
+      <c r="D79" s="28"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D80" s="14"/>
+      <c r="D80" s="28"/>
     </row>
     <row r="81" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D81" s="14"/>
+      <c r="D81" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="E47:E50"/>
+    <mergeCell ref="E3:E6"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="E11:E14"/>
+    <mergeCell ref="E15:E18"/>
+    <mergeCell ref="E19:E22"/>
+    <mergeCell ref="E23:E26"/>
+    <mergeCell ref="E27:E30"/>
+    <mergeCell ref="E31:E34"/>
+    <mergeCell ref="E35:E38"/>
+    <mergeCell ref="E39:E42"/>
+    <mergeCell ref="E43:E46"/>
     <mergeCell ref="F47:F50"/>
     <mergeCell ref="F3:F6"/>
     <mergeCell ref="F7:F10"/>
@@ -2695,18 +2723,6 @@
     <mergeCell ref="F35:F38"/>
     <mergeCell ref="F39:F42"/>
     <mergeCell ref="F43:F46"/>
-    <mergeCell ref="E47:E50"/>
-    <mergeCell ref="E3:E6"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="E11:E14"/>
-    <mergeCell ref="E15:E18"/>
-    <mergeCell ref="E19:E22"/>
-    <mergeCell ref="E23:E26"/>
-    <mergeCell ref="E27:E30"/>
-    <mergeCell ref="E31:E34"/>
-    <mergeCell ref="E35:E38"/>
-    <mergeCell ref="E39:E42"/>
-    <mergeCell ref="E43:E46"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75000000000000011" bottom="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>

</xml_diff>